<commit_message>
More classic evolutions, also updating some cards to have multiple types / Attributes.
</commit_message>
<xml_diff>
--- a/Custom Cards/Shortlist.xlsx
+++ b/Custom Cards/Shortlist.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\samhu\Documents\Documents\Game Design\Custom Yu-Gi-Oh! Cards\Custom Cards\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A536F223-2CDF-439D-B713-E2888CC79ABE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{510B304F-FE7E-4066-904F-59BB4C8751FA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="11520" yWindow="0" windowWidth="11520" windowHeight="12360" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -17,6 +17,7 @@
     <sheet name="Singles" sheetId="1" r:id="rId2"/>
   </sheets>
   <calcPr calcId="162913"/>
+  <fileRecoveryPr repairLoad="1"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -26,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="324" uniqueCount="78">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="384" uniqueCount="89">
   <si>
     <t>Format</t>
   </si>
@@ -260,6 +261,39 @@
   </si>
   <si>
     <t>Red-Eyes Archfiend Meteor Dragon</t>
+  </si>
+  <si>
+    <t>Shining Nova</t>
+  </si>
+  <si>
+    <t>Blue-Eyes</t>
+  </si>
+  <si>
+    <t>Dragon of a Thousand Years - Thousand Dragon</t>
+  </si>
+  <si>
+    <t>Metal Fiend Zoa</t>
+  </si>
+  <si>
+    <t>Great Cocoon of Evolution</t>
+  </si>
+  <si>
+    <t>Great Moth of Evolution</t>
+  </si>
+  <si>
+    <t>Larvae Moth of Evolution</t>
+  </si>
+  <si>
+    <t>Sage of a Thousand Years - Dark Sage</t>
+  </si>
+  <si>
+    <t>Triple Harpie Lady Sisters</t>
+  </si>
+  <si>
+    <t>Ultimate Moth of Evolution</t>
+  </si>
+  <si>
+    <t>Red-Eyes Zombie Evolution Dragon</t>
   </si>
 </sst>
 </file>
@@ -303,6 +337,34 @@
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="20">
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFFF00"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF00B050"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC000"/>
+        </patternFill>
+      </fill>
+    </dxf>
     <dxf>
       <fill>
         <patternFill>
@@ -430,34 +492,6 @@
       <fill>
         <patternFill>
           <bgColor rgb="FF002060"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF0000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFFF00"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF00B050"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC000"/>
         </patternFill>
       </fill>
     </dxf>
@@ -930,38 +964,38 @@
       </c>
     </row>
   </sheetData>
+  <conditionalFormatting sqref="A1">
+    <cfRule type="cellIs" dxfId="19" priority="2" operator="equal">
+      <formula>"Advanced Format"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="18" priority="3" operator="equal">
+      <formula>"HAT"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="17" priority="4" operator="equal">
+      <formula>"Tengu Plant"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="16" priority="5" operator="equal">
+      <formula>"Edison"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="15" priority="6" operator="equal">
+      <formula>"Gladiator"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="14" priority="7" operator="equal">
+      <formula>"Goat"</formula>
+    </cfRule>
+  </conditionalFormatting>
   <conditionalFormatting sqref="D1:F1">
-    <cfRule type="cellIs" dxfId="9" priority="1" operator="equal">
+    <cfRule type="cellIs" dxfId="13" priority="1" operator="equal">
       <formula>"Planned"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="8" priority="8" operator="equal">
+    <cfRule type="cellIs" dxfId="12" priority="8" operator="equal">
       <formula>"Complete"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="7" priority="9" operator="equal">
+    <cfRule type="cellIs" dxfId="11" priority="9" operator="equal">
       <formula>"In Progress"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="6" priority="10" operator="equal">
+    <cfRule type="cellIs" dxfId="10" priority="10" operator="equal">
       <formula>"Not Started"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="A1">
-    <cfRule type="cellIs" dxfId="5" priority="2" operator="equal">
-      <formula>"Advanced Format"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="4" priority="3" operator="equal">
-      <formula>"HAT"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="3" priority="4" operator="equal">
-      <formula>"Tengu Plant"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="2" priority="5" operator="equal">
-      <formula>"Edison"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="1" priority="6" operator="equal">
-      <formula>"Gladiator"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="0" priority="7" operator="equal">
-      <formula>"Goat"</formula>
     </cfRule>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -970,10 +1004,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:H45"/>
+  <dimension ref="A1:H55"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A28" workbookViewId="0">
-      <selection activeCell="D16" sqref="D16"/>
+    <sheetView tabSelected="1" topLeftCell="A22" workbookViewId="0">
+      <selection activeCell="D36" sqref="D36"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1023,7 +1057,7 @@
         <v>17</v>
       </c>
       <c r="D2" s="1">
-        <v>45819</v>
+        <v>45921</v>
       </c>
       <c r="E2" t="s">
         <v>8</v>
@@ -1276,7 +1310,7 @@
         <v>37</v>
       </c>
       <c r="D13" s="1">
-        <v>45843</v>
+        <v>45921</v>
       </c>
       <c r="E13" t="s">
         <v>8</v>
@@ -1483,7 +1517,7 @@
         <v>37</v>
       </c>
       <c r="D22" s="1">
-        <v>45843</v>
+        <v>45921</v>
       </c>
       <c r="E22" t="s">
         <v>8</v>
@@ -1805,7 +1839,7 @@
         <v>37</v>
       </c>
       <c r="D36" s="1">
-        <v>45742</v>
+        <v>45921</v>
       </c>
       <c r="E36" t="s">
         <v>8</v>
@@ -2024,39 +2058,269 @@
         <v>10</v>
       </c>
     </row>
+    <row r="46" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A46" t="s">
+        <v>4</v>
+      </c>
+      <c r="B46" t="s">
+        <v>78</v>
+      </c>
+      <c r="C46" t="s">
+        <v>79</v>
+      </c>
+      <c r="D46" s="1">
+        <v>45887</v>
+      </c>
+      <c r="E46" t="s">
+        <v>8</v>
+      </c>
+      <c r="F46" t="s">
+        <v>9</v>
+      </c>
+      <c r="G46" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="47" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A47" t="s">
+        <v>4</v>
+      </c>
+      <c r="B47" t="s">
+        <v>80</v>
+      </c>
+      <c r="C47" t="s">
+        <v>18</v>
+      </c>
+      <c r="D47" s="1">
+        <v>45920</v>
+      </c>
+      <c r="E47" t="s">
+        <v>8</v>
+      </c>
+      <c r="F47" t="s">
+        <v>10</v>
+      </c>
+      <c r="G47" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="48" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A48" t="s">
+        <v>4</v>
+      </c>
+      <c r="B48" t="s">
+        <v>85</v>
+      </c>
+      <c r="C48" t="s">
+        <v>18</v>
+      </c>
+      <c r="D48" s="1">
+        <v>45920</v>
+      </c>
+      <c r="E48" t="s">
+        <v>8</v>
+      </c>
+      <c r="F48" t="s">
+        <v>10</v>
+      </c>
+      <c r="G48" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="49" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A49" t="s">
+        <v>4</v>
+      </c>
+      <c r="B49" t="s">
+        <v>81</v>
+      </c>
+      <c r="C49" t="s">
+        <v>18</v>
+      </c>
+      <c r="D49" s="1">
+        <v>45920</v>
+      </c>
+      <c r="E49" t="s">
+        <v>8</v>
+      </c>
+      <c r="F49" t="s">
+        <v>10</v>
+      </c>
+      <c r="G49" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="50" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A50" t="s">
+        <v>4</v>
+      </c>
+      <c r="B50" t="s">
+        <v>82</v>
+      </c>
+      <c r="C50" t="s">
+        <v>18</v>
+      </c>
+      <c r="D50" s="1">
+        <v>45920</v>
+      </c>
+      <c r="E50" t="s">
+        <v>8</v>
+      </c>
+      <c r="F50" t="s">
+        <v>10</v>
+      </c>
+      <c r="G50" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="51" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A51" t="s">
+        <v>4</v>
+      </c>
+      <c r="B51" t="s">
+        <v>84</v>
+      </c>
+      <c r="C51" t="s">
+        <v>18</v>
+      </c>
+      <c r="D51" s="1">
+        <v>45920</v>
+      </c>
+      <c r="E51" t="s">
+        <v>8</v>
+      </c>
+      <c r="F51" t="s">
+        <v>10</v>
+      </c>
+      <c r="G51" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="52" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A52" t="s">
+        <v>4</v>
+      </c>
+      <c r="B52" t="s">
+        <v>83</v>
+      </c>
+      <c r="C52" t="s">
+        <v>18</v>
+      </c>
+      <c r="D52" s="1">
+        <v>45920</v>
+      </c>
+      <c r="E52" t="s">
+        <v>8</v>
+      </c>
+      <c r="F52" t="s">
+        <v>10</v>
+      </c>
+      <c r="G52" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="53" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A53" t="s">
+        <v>4</v>
+      </c>
+      <c r="B53" t="s">
+        <v>87</v>
+      </c>
+      <c r="C53" t="s">
+        <v>18</v>
+      </c>
+      <c r="D53" s="1">
+        <v>45920</v>
+      </c>
+      <c r="E53" t="s">
+        <v>8</v>
+      </c>
+      <c r="F53" t="s">
+        <v>10</v>
+      </c>
+      <c r="G53" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="54" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A54" t="s">
+        <v>4</v>
+      </c>
+      <c r="B54" t="s">
+        <v>86</v>
+      </c>
+      <c r="C54" t="s">
+        <v>18</v>
+      </c>
+      <c r="D54" s="1">
+        <v>45920</v>
+      </c>
+      <c r="E54" t="s">
+        <v>8</v>
+      </c>
+      <c r="F54" t="s">
+        <v>10</v>
+      </c>
+      <c r="G54" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="55" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A55" t="s">
+        <v>59</v>
+      </c>
+      <c r="B55" t="s">
+        <v>88</v>
+      </c>
+      <c r="C55" t="s">
+        <v>37</v>
+      </c>
+      <c r="D55" s="1">
+        <v>45921</v>
+      </c>
+      <c r="E55" t="s">
+        <v>8</v>
+      </c>
+      <c r="F55" t="s">
+        <v>10</v>
+      </c>
+      <c r="G55" t="s">
+        <v>10</v>
+      </c>
+    </row>
   </sheetData>
+  <conditionalFormatting sqref="A1:A1048576">
+    <cfRule type="cellIs" dxfId="9" priority="2" operator="equal">
+      <formula>"Advanced Format"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="8" priority="3" operator="equal">
+      <formula>"HAT"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="7" priority="4" operator="equal">
+      <formula>"Tengu Plant"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="6" priority="5" operator="equal">
+      <formula>"Edison"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="5" priority="6" operator="equal">
+      <formula>"Gladiator"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="4" priority="7" operator="equal">
+      <formula>"Goat"</formula>
+    </cfRule>
+  </conditionalFormatting>
   <conditionalFormatting sqref="E1:G1048576">
-    <cfRule type="cellIs" dxfId="19" priority="1" operator="equal">
+    <cfRule type="cellIs" dxfId="3" priority="1" operator="equal">
       <formula>"Planned"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="18" priority="8" operator="equal">
+    <cfRule type="cellIs" dxfId="2" priority="8" operator="equal">
       <formula>"Complete"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="17" priority="9" operator="equal">
+    <cfRule type="cellIs" dxfId="1" priority="9" operator="equal">
       <formula>"In Progress"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="16" priority="10" operator="equal">
+    <cfRule type="cellIs" dxfId="0" priority="10" operator="equal">
       <formula>"Not Started"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="A1:A1048576">
-    <cfRule type="cellIs" dxfId="15" priority="2" operator="equal">
-      <formula>"Advanced Format"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="14" priority="3" operator="equal">
-      <formula>"HAT"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="13" priority="4" operator="equal">
-      <formula>"Tengu Plant"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="12" priority="5" operator="equal">
-      <formula>"Edison"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="11" priority="6" operator="equal">
-      <formula>"Gladiator"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="10" priority="7" operator="equal">
-      <formula>"Goat"</formula>
     </cfRule>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Idea for Red-Eyes Zombie Dragon if Evolution Monsters had existed.
</commit_message>
<xml_diff>
--- a/Custom Cards/Shortlist.xlsx
+++ b/Custom Cards/Shortlist.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\samhu\Documents\Documents\Game Design\Custom Yu-Gi-Oh! Cards\Custom Cards\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{510B304F-FE7E-4066-904F-59BB4C8751FA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FDD29EB1-D73F-47D4-8FEA-C110D8A686C4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="11520" yWindow="0" windowWidth="11520" windowHeight="12360" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -17,7 +17,6 @@
     <sheet name="Singles" sheetId="1" r:id="rId2"/>
   </sheets>
   <calcPr calcId="162913"/>
-  <fileRecoveryPr repairLoad="1"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -1006,8 +1005,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:H55"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A22" workbookViewId="0">
-      <selection activeCell="D36" sqref="D36"/>
+    <sheetView tabSelected="1" topLeftCell="A43" workbookViewId="0">
+      <selection activeCell="F55" sqref="F55"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2282,7 +2281,7 @@
         <v>8</v>
       </c>
       <c r="F55" t="s">
-        <v>10</v>
+        <v>38</v>
       </c>
       <c r="G55" t="s">
         <v>10</v>

</xml_diff>

<commit_message>
Updated the singles shortlist.
</commit_message>
<xml_diff>
--- a/Custom Cards/Shortlist.xlsx
+++ b/Custom Cards/Shortlist.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\samhu\Documents\Documents\Game Design\Custom Yu-Gi-Oh! Cards\Custom Cards\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FDD29EB1-D73F-47D4-8FEA-C110D8A686C4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{868E30BF-8A11-4428-961F-0709D41612BA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="11520" yWindow="0" windowWidth="11520" windowHeight="12360" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Themes" sheetId="2" r:id="rId1"/>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="384" uniqueCount="89">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="394" uniqueCount="90">
   <si>
     <t>Format</t>
   </si>
@@ -52,9 +52,6 @@
     <t>Blue-Eyes Shining Evolution Dragon</t>
   </si>
   <si>
-    <t>Complete</t>
-  </si>
-  <si>
     <t>In Progress</t>
   </si>
   <si>
@@ -293,6 +290,12 @@
   </si>
   <si>
     <t>Red-Eyes Zombie Evolution Dragon</t>
+  </si>
+  <si>
+    <t>Multi-Attribute monsters</t>
+  </si>
+  <si>
+    <t>Lycanthrope</t>
   </si>
 </sst>
 </file>
@@ -335,32 +338,32 @@
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="20">
+  <dxfs count="128">
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF00B050"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFFF00"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC000"/>
+        </patternFill>
+      </fill>
+    </dxf>
     <dxf>
       <fill>
         <patternFill>
           <bgColor rgb="FFFF0000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFFF00"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF00B050"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC000"/>
         </patternFill>
       </fill>
     </dxf>
@@ -412,6 +415,816 @@
       <fill>
         <patternFill>
           <bgColor rgb="FF002060"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFFF00"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF00B050"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF00B0F0"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="0"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF7030A0"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="0" tint="-0.14996795556505021"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="0" tint="-0.34998626667073579"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="0"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor theme="1"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="0"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF002060"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFFF00"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF00B050"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF00B0F0"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="0"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF7030A0"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="0" tint="-0.14996795556505021"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="0" tint="-0.34998626667073579"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="0"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor theme="1"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="0"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF002060"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFFF00"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF00B050"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFFF00"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF00B050"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFFF00"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF00B050"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFFF00"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF00B050"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFFF00"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF00B050"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFFF00"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF00B050"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFFF00"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF00B050"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF00B0F0"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="0"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF7030A0"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="0" tint="-0.14996795556505021"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="0" tint="-0.34998626667073579"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="0"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor theme="1"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="0"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF002060"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFFF00"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF00B050"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFFF00"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF00B050"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFFF00"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF00B050"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFFF00"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF00B050"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFFF00"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF00B050"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFFF00"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF00B050"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFFF00"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF00B050"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF00B0F0"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="0"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF7030A0"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="0" tint="-0.14996795556505021"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="0" tint="-0.34998626667073579"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="0"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor theme="1"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="0"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF002060"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF00B0F0"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="0"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF7030A0"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="0" tint="-0.14996795556505021"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="0" tint="-0.34998626667073579"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="0"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor theme="1"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="0"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF002060"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFFF00"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF00B050"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="0"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF002060"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFFF00"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF00B050"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF00B0F0"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="0"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF7030A0"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="0" tint="-0.14996795556505021"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="0" tint="-0.34998626667073579"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="0"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor theme="1"/>
         </patternFill>
       </fill>
     </dxf>
@@ -770,20 +1583,21 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C2E7FF8C-8C53-469D-A4DC-477B6EEC4FE3}">
-  <dimension ref="A1:G10"/>
+  <dimension ref="A1:G12"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A11" sqref="A11"/>
+      <selection activeCell="J4" sqref="J4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="8.5546875" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="20.5546875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="25.44140625" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="13.88671875" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="11.33203125" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="11.33203125" customWidth="1"/>
     <col min="6" max="6" width="10.44140625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="9.77734375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.3">
@@ -791,16 +1605,16 @@
         <v>0</v>
       </c>
       <c r="B1" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="C1" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="D1" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="E1" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="F1" t="s">
         <v>2</v>
@@ -811,33 +1625,33 @@
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
+        <v>49</v>
+      </c>
+      <c r="B2" t="s">
         <v>55</v>
       </c>
-      <c r="B2" t="s">
-        <v>36</v>
-      </c>
       <c r="D2" t="s">
-        <v>9</v>
+        <v>56</v>
       </c>
       <c r="E2" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F2" t="s">
-        <v>10</v>
+        <v>56</v>
       </c>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
-        <v>50</v>
+        <v>4</v>
       </c>
       <c r="B3" t="s">
-        <v>56</v>
+        <v>88</v>
       </c>
       <c r="D3" t="s">
-        <v>8</v>
+        <v>56</v>
       </c>
       <c r="E3" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F3" t="s">
         <v>8</v>
@@ -848,122 +1662,163 @@
         <v>4</v>
       </c>
       <c r="B4" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="D4" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="E4" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F4" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="B5" t="s">
-        <v>61</v>
+        <v>89</v>
       </c>
       <c r="D5" t="s">
-        <v>9</v>
+        <v>56</v>
       </c>
       <c r="E5" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F5" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="B6" t="s">
-        <v>62</v>
+        <v>64</v>
       </c>
       <c r="D6" t="s">
-        <v>9</v>
+        <v>56</v>
       </c>
       <c r="E6" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F6" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
-        <v>55</v>
+        <v>71</v>
       </c>
       <c r="B7" t="s">
-        <v>63</v>
+        <v>72</v>
       </c>
       <c r="D7" t="s">
-        <v>10</v>
+        <v>56</v>
       </c>
       <c r="E7" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F7" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="B8" t="s">
-        <v>64</v>
+        <v>60</v>
       </c>
       <c r="D8" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="E8" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F8" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="B9" t="s">
-        <v>65</v>
+        <v>61</v>
       </c>
       <c r="D9" t="s">
-        <v>57</v>
+        <v>8</v>
       </c>
       <c r="E9" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F9" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
-        <v>72</v>
+        <v>54</v>
       </c>
       <c r="B10" t="s">
-        <v>73</v>
+        <v>35</v>
       </c>
       <c r="D10" t="s">
-        <v>57</v>
+        <v>8</v>
       </c>
       <c r="E10" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F10" t="s">
-        <v>10</v>
+        <v>9</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A11" t="s">
+        <v>54</v>
+      </c>
+      <c r="B11" t="s">
+        <v>63</v>
+      </c>
+      <c r="D11" t="s">
+        <v>9</v>
+      </c>
+      <c r="E11" t="s">
+        <v>9</v>
+      </c>
+      <c r="F11" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="12" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A12" t="s">
+        <v>54</v>
+      </c>
+      <c r="B12" t="s">
+        <v>62</v>
+      </c>
+      <c r="D12" t="s">
+        <v>9</v>
+      </c>
+      <c r="E12" t="s">
+        <v>9</v>
+      </c>
+      <c r="F12" t="s">
+        <v>9</v>
       </c>
     </row>
   </sheetData>
-  <conditionalFormatting sqref="A1">
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:G14">
+    <sortCondition ref="D2:D14" customList="Done,In Progress,Planned,Not Started"/>
+    <sortCondition descending="1" ref="E2:E14" customList="Not Started,In Progress,Done"/>
+    <sortCondition descending="1" ref="F2:F14" customList="Not Started,In Progress,Done"/>
+    <sortCondition ref="A2:A14" customList="Goat,Gladiator,Edison,Tengu Plant,HAT,Advanced"/>
+    <sortCondition ref="B2:B14"/>
+  </sortState>
+  <conditionalFormatting sqref="A1:A1048576">
     <cfRule type="cellIs" dxfId="19" priority="2" operator="equal">
       <formula>"Advanced Format"</formula>
     </cfRule>
@@ -983,12 +1838,12 @@
       <formula>"Goat"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="D1:F1">
+  <conditionalFormatting sqref="D1:F1048576">
     <cfRule type="cellIs" dxfId="13" priority="1" operator="equal">
       <formula>"Planned"</formula>
     </cfRule>
     <cfRule type="cellIs" dxfId="12" priority="8" operator="equal">
-      <formula>"Complete"</formula>
+      <formula>"Done"</formula>
     </cfRule>
     <cfRule type="cellIs" dxfId="11" priority="9" operator="equal">
       <formula>"In Progress"</formula>
@@ -1005,9 +1860,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:H55"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A43" workbookViewId="0">
-      <selection activeCell="F55" sqref="F55"/>
-    </sheetView>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
@@ -1017,6 +1870,7 @@
     <col min="4" max="4" width="13.88671875" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="11.33203125" bestFit="1" customWidth="1"/>
     <col min="6" max="7" width="10.44140625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="9.77734375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:8" x14ac:dyDescent="0.3">
@@ -1027,19 +1881,19 @@
         <v>1</v>
       </c>
       <c r="C1" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="D1" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="E1" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="F1" t="s">
+        <v>10</v>
+      </c>
+      <c r="G1" t="s">
         <v>2</v>
-      </c>
-      <c r="G1" t="s">
-        <v>11</v>
       </c>
       <c r="H1" t="s">
         <v>3</v>
@@ -1047,25 +1901,25 @@
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
-        <v>4</v>
+        <v>58</v>
       </c>
       <c r="B2" t="s">
-        <v>5</v>
+        <v>59</v>
       </c>
       <c r="C2" t="s">
-        <v>17</v>
+        <v>36</v>
       </c>
       <c r="D2" s="1">
         <v>45921</v>
       </c>
       <c r="E2" t="s">
-        <v>8</v>
+        <v>56</v>
       </c>
       <c r="F2" t="s">
         <v>9</v>
       </c>
       <c r="G2" t="s">
-        <v>10</v>
+        <v>56</v>
       </c>
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.3">
@@ -1073,22 +1927,22 @@
         <v>4</v>
       </c>
       <c r="B3" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="C3" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="D3" s="1">
-        <v>45826</v>
+        <v>45921</v>
       </c>
       <c r="E3" t="s">
+        <v>56</v>
+      </c>
+      <c r="F3" t="s">
+        <v>9</v>
+      </c>
+      <c r="G3" t="s">
         <v>8</v>
-      </c>
-      <c r="F3" t="s">
-        <v>9</v>
-      </c>
-      <c r="G3" t="s">
-        <v>10</v>
       </c>
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.3">
@@ -1096,22 +1950,22 @@
         <v>4</v>
       </c>
       <c r="B4" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="C4" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="D4" s="1">
-        <v>45887</v>
+        <v>45826</v>
       </c>
       <c r="E4" t="s">
+        <v>56</v>
+      </c>
+      <c r="F4" t="s">
+        <v>9</v>
+      </c>
+      <c r="G4" t="s">
         <v>8</v>
-      </c>
-      <c r="F4" t="s">
-        <v>10</v>
-      </c>
-      <c r="G4" t="s">
-        <v>10</v>
       </c>
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.3">
@@ -1119,22 +1973,22 @@
         <v>4</v>
       </c>
       <c r="B5" t="s">
-        <v>13</v>
+        <v>77</v>
       </c>
       <c r="C5" t="s">
-        <v>17</v>
+        <v>78</v>
       </c>
       <c r="D5" s="1">
-        <v>45867</v>
+        <v>45887</v>
       </c>
       <c r="E5" t="s">
+        <v>56</v>
+      </c>
+      <c r="F5" t="s">
+        <v>9</v>
+      </c>
+      <c r="G5" t="s">
         <v>8</v>
-      </c>
-      <c r="F5" t="s">
-        <v>10</v>
-      </c>
-      <c r="G5" t="s">
-        <v>10</v>
       </c>
     </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.3">
@@ -1142,22 +1996,22 @@
         <v>4</v>
       </c>
       <c r="B6" t="s">
-        <v>14</v>
+        <v>25</v>
       </c>
       <c r="C6" t="s">
-        <v>17</v>
+        <v>36</v>
       </c>
       <c r="D6" s="1">
-        <v>45822</v>
+        <v>45921</v>
       </c>
       <c r="E6" t="s">
-        <v>9</v>
+        <v>56</v>
       </c>
       <c r="F6" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="G6" t="s">
-        <v>10</v>
+        <v>37</v>
       </c>
     </row>
     <row r="7" spans="1:8" x14ac:dyDescent="0.3">
@@ -1165,22 +2019,22 @@
         <v>4</v>
       </c>
       <c r="B7" t="s">
-        <v>15</v>
+        <v>28</v>
       </c>
       <c r="C7" t="s">
-        <v>17</v>
+        <v>36</v>
       </c>
       <c r="D7" s="1">
-        <v>45822</v>
+        <v>45920</v>
       </c>
       <c r="E7" t="s">
-        <v>8</v>
+        <v>56</v>
       </c>
       <c r="F7" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="G7" t="s">
-        <v>10</v>
+        <v>37</v>
       </c>
     </row>
     <row r="8" spans="1:8" x14ac:dyDescent="0.3">
@@ -1188,22 +2042,22 @@
         <v>4</v>
       </c>
       <c r="B8" t="s">
-        <v>20</v>
+        <v>29</v>
       </c>
       <c r="C8" t="s">
-        <v>21</v>
+        <v>36</v>
       </c>
       <c r="D8" s="1">
-        <v>45800</v>
+        <v>45920</v>
       </c>
       <c r="E8" t="s">
-        <v>9</v>
+        <v>56</v>
       </c>
       <c r="F8" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="G8" t="s">
-        <v>10</v>
+        <v>37</v>
       </c>
     </row>
     <row r="9" spans="1:8" x14ac:dyDescent="0.3">
@@ -1211,137 +2065,137 @@
         <v>4</v>
       </c>
       <c r="B9" t="s">
-        <v>22</v>
+        <v>34</v>
       </c>
       <c r="C9" t="s">
-        <v>21</v>
+        <v>36</v>
       </c>
       <c r="D9" s="1">
-        <v>45800</v>
+        <v>45921</v>
       </c>
       <c r="E9" t="s">
-        <v>9</v>
+        <v>56</v>
       </c>
       <c r="F9" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="G9" t="s">
-        <v>10</v>
+        <v>37</v>
       </c>
     </row>
     <row r="10" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
-        <v>4</v>
+        <v>58</v>
       </c>
       <c r="B10" t="s">
-        <v>23</v>
+        <v>87</v>
       </c>
       <c r="C10" t="s">
-        <v>18</v>
+        <v>36</v>
       </c>
       <c r="D10" s="1">
-        <v>45887</v>
+        <v>45921</v>
       </c>
       <c r="E10" t="s">
-        <v>8</v>
+        <v>56</v>
       </c>
       <c r="F10" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="G10" t="s">
-        <v>10</v>
+        <v>37</v>
       </c>
     </row>
     <row r="11" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
-        <v>4</v>
+        <v>71</v>
       </c>
       <c r="B11" t="s">
-        <v>24</v>
+        <v>73</v>
       </c>
       <c r="C11" t="s">
-        <v>18</v>
+        <v>51</v>
       </c>
       <c r="D11" s="1">
-        <v>45887</v>
+        <v>45879</v>
       </c>
       <c r="E11" t="s">
-        <v>8</v>
+        <v>56</v>
       </c>
       <c r="F11" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="G11" t="s">
-        <v>10</v>
+        <v>37</v>
       </c>
     </row>
     <row r="12" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
-        <v>4</v>
+        <v>71</v>
       </c>
       <c r="B12" t="s">
-        <v>25</v>
+        <v>74</v>
       </c>
       <c r="C12" t="s">
+        <v>51</v>
+      </c>
+      <c r="D12" s="1">
+        <v>45815</v>
+      </c>
+      <c r="E12" t="s">
+        <v>56</v>
+      </c>
+      <c r="F12" t="s">
+        <v>9</v>
+      </c>
+      <c r="G12" t="s">
         <v>37</v>
-      </c>
-      <c r="D12" s="1">
-        <v>45910</v>
-      </c>
-      <c r="E12" t="s">
-        <v>8</v>
-      </c>
-      <c r="F12" t="s">
-        <v>10</v>
-      </c>
-      <c r="G12" t="s">
-        <v>10</v>
       </c>
     </row>
     <row r="13" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
-        <v>4</v>
+        <v>71</v>
       </c>
       <c r="B13" t="s">
-        <v>26</v>
+        <v>75</v>
       </c>
       <c r="C13" t="s">
+        <v>51</v>
+      </c>
+      <c r="D13" s="1">
+        <v>45879</v>
+      </c>
+      <c r="E13" t="s">
+        <v>56</v>
+      </c>
+      <c r="F13" t="s">
+        <v>9</v>
+      </c>
+      <c r="G13" t="s">
         <v>37</v>
-      </c>
-      <c r="D13" s="1">
-        <v>45921</v>
-      </c>
-      <c r="E13" t="s">
-        <v>8</v>
-      </c>
-      <c r="F13" t="s">
-        <v>38</v>
-      </c>
-      <c r="G13" t="s">
-        <v>10</v>
       </c>
     </row>
     <row r="14" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
-        <v>4</v>
+        <v>71</v>
       </c>
       <c r="B14" t="s">
-        <v>27</v>
+        <v>76</v>
       </c>
       <c r="C14" t="s">
+        <v>51</v>
+      </c>
+      <c r="D14" s="1">
+        <v>45879</v>
+      </c>
+      <c r="E14" t="s">
+        <v>56</v>
+      </c>
+      <c r="F14" t="s">
+        <v>9</v>
+      </c>
+      <c r="G14" t="s">
         <v>37</v>
-      </c>
-      <c r="D14" s="1">
-        <v>45919</v>
-      </c>
-      <c r="E14" t="s">
-        <v>8</v>
-      </c>
-      <c r="F14" t="s">
-        <v>10</v>
-      </c>
-      <c r="G14" t="s">
-        <v>10</v>
       </c>
     </row>
     <row r="15" spans="1:8" x14ac:dyDescent="0.3">
@@ -1349,22 +2203,22 @@
         <v>4</v>
       </c>
       <c r="B15" t="s">
-        <v>28</v>
+        <v>7</v>
       </c>
       <c r="C15" t="s">
-        <v>36</v>
+        <v>17</v>
       </c>
       <c r="D15" s="1">
-        <v>45835</v>
+        <v>45887</v>
       </c>
       <c r="E15" t="s">
-        <v>8</v>
+        <v>56</v>
       </c>
       <c r="F15" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="G15" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
     </row>
     <row r="16" spans="1:8" x14ac:dyDescent="0.3">
@@ -1372,22 +2226,22 @@
         <v>4</v>
       </c>
       <c r="B16" t="s">
-        <v>29</v>
+        <v>24</v>
       </c>
       <c r="C16" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="D16" s="1">
-        <v>45920</v>
+        <v>45910</v>
       </c>
       <c r="E16" t="s">
-        <v>8</v>
+        <v>56</v>
       </c>
       <c r="F16" t="s">
-        <v>38</v>
+        <v>9</v>
       </c>
       <c r="G16" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
     </row>
     <row r="17" spans="1:7" x14ac:dyDescent="0.3">
@@ -1395,22 +2249,22 @@
         <v>4</v>
       </c>
       <c r="B17" t="s">
-        <v>30</v>
+        <v>26</v>
       </c>
       <c r="C17" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="D17" s="1">
-        <v>45920</v>
+        <v>45919</v>
       </c>
       <c r="E17" t="s">
-        <v>8</v>
+        <v>56</v>
       </c>
       <c r="F17" t="s">
-        <v>38</v>
+        <v>9</v>
       </c>
       <c r="G17" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
     </row>
     <row r="18" spans="1:7" x14ac:dyDescent="0.3">
@@ -1418,22 +2272,22 @@
         <v>4</v>
       </c>
       <c r="B18" t="s">
-        <v>31</v>
+        <v>79</v>
       </c>
       <c r="C18" t="s">
-        <v>37</v>
+        <v>17</v>
       </c>
       <c r="D18" s="1">
-        <v>45800</v>
+        <v>45920</v>
       </c>
       <c r="E18" t="s">
-        <v>8</v>
+        <v>56</v>
       </c>
       <c r="F18" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="G18" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
     </row>
     <row r="19" spans="1:7" x14ac:dyDescent="0.3">
@@ -1441,22 +2295,22 @@
         <v>4</v>
       </c>
       <c r="B19" t="s">
-        <v>32</v>
+        <v>27</v>
       </c>
       <c r="C19" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="D19" s="1">
-        <v>45907</v>
+        <v>45835</v>
       </c>
       <c r="E19" t="s">
-        <v>8</v>
+        <v>56</v>
       </c>
       <c r="F19" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="G19" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
     </row>
     <row r="20" spans="1:7" x14ac:dyDescent="0.3">
@@ -1464,22 +2318,22 @@
         <v>4</v>
       </c>
       <c r="B20" t="s">
-        <v>33</v>
+        <v>12</v>
       </c>
       <c r="C20" t="s">
-        <v>37</v>
+        <v>16</v>
       </c>
       <c r="D20" s="1">
-        <v>45919</v>
+        <v>45867</v>
       </c>
       <c r="E20" t="s">
-        <v>8</v>
+        <v>56</v>
       </c>
       <c r="F20" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="G20" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
     </row>
     <row r="21" spans="1:7" x14ac:dyDescent="0.3">
@@ -1487,22 +2341,22 @@
         <v>4</v>
       </c>
       <c r="B21" t="s">
-        <v>34</v>
+        <v>81</v>
       </c>
       <c r="C21" t="s">
-        <v>37</v>
+        <v>17</v>
       </c>
       <c r="D21" s="1">
-        <v>45910</v>
+        <v>45920</v>
       </c>
       <c r="E21" t="s">
-        <v>8</v>
+        <v>56</v>
       </c>
       <c r="F21" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="G21" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
     </row>
     <row r="22" spans="1:7" x14ac:dyDescent="0.3">
@@ -1510,22 +2364,22 @@
         <v>4</v>
       </c>
       <c r="B22" t="s">
-        <v>35</v>
+        <v>82</v>
       </c>
       <c r="C22" t="s">
-        <v>37</v>
+        <v>17</v>
       </c>
       <c r="D22" s="1">
-        <v>45921</v>
+        <v>45920</v>
       </c>
       <c r="E22" t="s">
-        <v>8</v>
+        <v>56</v>
       </c>
       <c r="F22" t="s">
-        <v>38</v>
+        <v>9</v>
       </c>
       <c r="G22" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
     </row>
     <row r="23" spans="1:7" x14ac:dyDescent="0.3">
@@ -1533,22 +2387,22 @@
         <v>4</v>
       </c>
       <c r="B23" t="s">
-        <v>39</v>
+        <v>83</v>
       </c>
       <c r="C23" t="s">
-        <v>49</v>
+        <v>17</v>
       </c>
       <c r="D23" s="1">
-        <v>45891</v>
+        <v>45920</v>
       </c>
       <c r="E23" t="s">
-        <v>9</v>
+        <v>56</v>
       </c>
       <c r="F23" t="s">
-        <v>38</v>
+        <v>9</v>
       </c>
       <c r="G23" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
     </row>
     <row r="24" spans="1:7" x14ac:dyDescent="0.3">
@@ -1556,22 +2410,22 @@
         <v>4</v>
       </c>
       <c r="B24" t="s">
-        <v>40</v>
+        <v>30</v>
       </c>
       <c r="C24" t="s">
-        <v>49</v>
+        <v>36</v>
       </c>
       <c r="D24" s="1">
-        <v>45891</v>
+        <v>45800</v>
       </c>
       <c r="E24" t="s">
-        <v>9</v>
+        <v>56</v>
       </c>
       <c r="F24" t="s">
-        <v>38</v>
+        <v>9</v>
       </c>
       <c r="G24" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
     </row>
     <row r="25" spans="1:7" x14ac:dyDescent="0.3">
@@ -1579,22 +2433,22 @@
         <v>4</v>
       </c>
       <c r="B25" t="s">
-        <v>41</v>
+        <v>80</v>
       </c>
       <c r="C25" t="s">
-        <v>49</v>
+        <v>17</v>
       </c>
       <c r="D25" s="1">
-        <v>45891</v>
+        <v>45920</v>
       </c>
       <c r="E25" t="s">
-        <v>9</v>
+        <v>56</v>
       </c>
       <c r="F25" t="s">
-        <v>38</v>
+        <v>9</v>
       </c>
       <c r="G25" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
     </row>
     <row r="26" spans="1:7" x14ac:dyDescent="0.3">
@@ -1602,22 +2456,22 @@
         <v>4</v>
       </c>
       <c r="B26" t="s">
-        <v>42</v>
+        <v>31</v>
       </c>
       <c r="C26" t="s">
-        <v>49</v>
+        <v>35</v>
       </c>
       <c r="D26" s="1">
-        <v>45891</v>
+        <v>45907</v>
       </c>
       <c r="E26" t="s">
-        <v>9</v>
+        <v>56</v>
       </c>
       <c r="F26" t="s">
-        <v>38</v>
+        <v>9</v>
       </c>
       <c r="G26" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
     </row>
     <row r="27" spans="1:7" x14ac:dyDescent="0.3">
@@ -1625,22 +2479,22 @@
         <v>4</v>
       </c>
       <c r="B27" t="s">
-        <v>43</v>
+        <v>22</v>
       </c>
       <c r="C27" t="s">
-        <v>49</v>
+        <v>17</v>
       </c>
       <c r="D27" s="1">
-        <v>45891</v>
+        <v>45887</v>
       </c>
       <c r="E27" t="s">
-        <v>9</v>
+        <v>56</v>
       </c>
       <c r="F27" t="s">
         <v>9</v>
       </c>
       <c r="G27" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
     </row>
     <row r="28" spans="1:7" x14ac:dyDescent="0.3">
@@ -1648,22 +2502,22 @@
         <v>4</v>
       </c>
       <c r="B28" t="s">
-        <v>44</v>
+        <v>23</v>
       </c>
       <c r="C28" t="s">
-        <v>49</v>
+        <v>17</v>
       </c>
       <c r="D28" s="1">
-        <v>45891</v>
+        <v>45887</v>
       </c>
       <c r="E28" t="s">
-        <v>9</v>
+        <v>56</v>
       </c>
       <c r="F28" t="s">
-        <v>38</v>
+        <v>9</v>
       </c>
       <c r="G28" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
     </row>
     <row r="29" spans="1:7" x14ac:dyDescent="0.3">
@@ -1671,22 +2525,22 @@
         <v>4</v>
       </c>
       <c r="B29" t="s">
-        <v>45</v>
+        <v>84</v>
       </c>
       <c r="C29" t="s">
-        <v>49</v>
+        <v>17</v>
       </c>
       <c r="D29" s="1">
-        <v>45891</v>
+        <v>45920</v>
       </c>
       <c r="E29" t="s">
-        <v>9</v>
+        <v>56</v>
       </c>
       <c r="F29" t="s">
-        <v>38</v>
+        <v>9</v>
       </c>
       <c r="G29" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
     </row>
     <row r="30" spans="1:7" x14ac:dyDescent="0.3">
@@ -1694,22 +2548,22 @@
         <v>4</v>
       </c>
       <c r="B30" t="s">
-        <v>46</v>
+        <v>14</v>
       </c>
       <c r="C30" t="s">
-        <v>49</v>
+        <v>16</v>
       </c>
       <c r="D30" s="1">
-        <v>45891</v>
+        <v>45822</v>
       </c>
       <c r="E30" t="s">
-        <v>9</v>
+        <v>56</v>
       </c>
       <c r="F30" t="s">
-        <v>38</v>
+        <v>9</v>
       </c>
       <c r="G30" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
     </row>
     <row r="31" spans="1:7" x14ac:dyDescent="0.3">
@@ -1717,22 +2571,22 @@
         <v>4</v>
       </c>
       <c r="B31" t="s">
-        <v>47</v>
+        <v>85</v>
       </c>
       <c r="C31" t="s">
-        <v>49</v>
+        <v>17</v>
       </c>
       <c r="D31" s="1">
-        <v>45891</v>
+        <v>45920</v>
       </c>
       <c r="E31" t="s">
-        <v>9</v>
+        <v>56</v>
       </c>
       <c r="F31" t="s">
-        <v>38</v>
+        <v>9</v>
       </c>
       <c r="G31" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
     </row>
     <row r="32" spans="1:7" x14ac:dyDescent="0.3">
@@ -1740,321 +2594,321 @@
         <v>4</v>
       </c>
       <c r="B32" t="s">
-        <v>48</v>
+        <v>32</v>
       </c>
       <c r="C32" t="s">
-        <v>49</v>
+        <v>36</v>
       </c>
       <c r="D32" s="1">
-        <v>45891</v>
+        <v>45919</v>
       </c>
       <c r="E32" t="s">
-        <v>9</v>
+        <v>56</v>
       </c>
       <c r="F32" t="s">
-        <v>38</v>
+        <v>9</v>
       </c>
       <c r="G32" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
     </row>
     <row r="33" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A33" t="s">
-        <v>50</v>
+        <v>4</v>
       </c>
       <c r="B33" t="s">
-        <v>51</v>
+        <v>86</v>
       </c>
       <c r="C33" t="s">
-        <v>52</v>
+        <v>17</v>
       </c>
       <c r="D33" s="1">
-        <v>45887</v>
+        <v>45920</v>
       </c>
       <c r="E33" t="s">
-        <v>8</v>
+        <v>56</v>
       </c>
       <c r="F33" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="G33" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
     </row>
     <row r="34" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A34" t="s">
-        <v>50</v>
+        <v>4</v>
       </c>
       <c r="B34" t="s">
-        <v>53</v>
+        <v>33</v>
       </c>
       <c r="C34" t="s">
-        <v>17</v>
+        <v>36</v>
       </c>
       <c r="D34" s="1">
-        <v>45819</v>
+        <v>45910</v>
       </c>
       <c r="E34" t="s">
-        <v>8</v>
+        <v>56</v>
       </c>
       <c r="F34" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="G34" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
     </row>
     <row r="35" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A35" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="B35" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="C35" t="s">
-        <v>37</v>
+        <v>16</v>
       </c>
       <c r="D35" s="1">
-        <v>45753</v>
+        <v>45819</v>
       </c>
       <c r="E35" t="s">
-        <v>8</v>
+        <v>56</v>
       </c>
       <c r="F35" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="G35" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
     </row>
     <row r="36" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A36" t="s">
-        <v>59</v>
+        <v>49</v>
       </c>
       <c r="B36" t="s">
-        <v>60</v>
+        <v>53</v>
       </c>
       <c r="C36" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="D36" s="1">
-        <v>45921</v>
+        <v>45753</v>
       </c>
       <c r="E36" t="s">
-        <v>8</v>
+        <v>56</v>
       </c>
       <c r="F36" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="G36" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
     </row>
     <row r="37" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A37" t="s">
-        <v>55</v>
+        <v>49</v>
       </c>
       <c r="B37" t="s">
-        <v>66</v>
+        <v>50</v>
       </c>
       <c r="C37" t="s">
-        <v>68</v>
+        <v>51</v>
       </c>
       <c r="D37" s="1">
-        <v>45787</v>
+        <v>45887</v>
       </c>
       <c r="E37" t="s">
-        <v>8</v>
+        <v>56</v>
       </c>
       <c r="F37" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="G37" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
     </row>
     <row r="38" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A38" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="B38" t="s">
+        <v>68</v>
+      </c>
+      <c r="C38" t="s">
         <v>67</v>
-      </c>
-      <c r="C38" t="s">
-        <v>68</v>
       </c>
       <c r="D38" s="1">
         <v>45787</v>
       </c>
       <c r="E38" t="s">
-        <v>8</v>
+        <v>56</v>
       </c>
       <c r="F38" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="G38" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
     </row>
     <row r="39" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A39" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="B39" t="s">
         <v>69</v>
       </c>
       <c r="C39" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="D39" s="1">
-        <v>45787</v>
+        <v>45786</v>
       </c>
       <c r="E39" t="s">
-        <v>8</v>
+        <v>56</v>
       </c>
       <c r="F39" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="G39" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
     </row>
     <row r="40" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A40" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="B40" t="s">
-        <v>70</v>
+        <v>66</v>
       </c>
       <c r="C40" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="D40" s="1">
-        <v>45786</v>
+        <v>45787</v>
       </c>
       <c r="E40" t="s">
-        <v>8</v>
+        <v>56</v>
       </c>
       <c r="F40" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="G40" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
     </row>
     <row r="41" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A41" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="B41" t="s">
-        <v>71</v>
+        <v>65</v>
       </c>
       <c r="C41" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="D41" s="1">
         <v>45787</v>
       </c>
       <c r="E41" t="s">
-        <v>8</v>
+        <v>56</v>
       </c>
       <c r="F41" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="G41" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
     </row>
     <row r="42" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A42" t="s">
-        <v>72</v>
+        <v>54</v>
       </c>
       <c r="B42" t="s">
-        <v>74</v>
+        <v>70</v>
       </c>
       <c r="C42" t="s">
-        <v>52</v>
+        <v>67</v>
       </c>
       <c r="D42" s="1">
-        <v>45879</v>
+        <v>45787</v>
       </c>
       <c r="E42" t="s">
-        <v>8</v>
+        <v>56</v>
       </c>
       <c r="F42" t="s">
-        <v>38</v>
+        <v>9</v>
       </c>
       <c r="G42" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
     </row>
     <row r="43" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A43" t="s">
-        <v>72</v>
+        <v>4</v>
       </c>
       <c r="B43" t="s">
-        <v>75</v>
+        <v>21</v>
       </c>
       <c r="C43" t="s">
-        <v>52</v>
+        <v>20</v>
       </c>
       <c r="D43" s="1">
-        <v>45815</v>
+        <v>45800</v>
       </c>
       <c r="E43" t="s">
         <v>8</v>
       </c>
       <c r="F43" t="s">
-        <v>38</v>
+        <v>9</v>
       </c>
       <c r="G43" t="s">
-        <v>10</v>
+        <v>56</v>
       </c>
     </row>
     <row r="44" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A44" t="s">
-        <v>72</v>
+        <v>4</v>
       </c>
       <c r="B44" t="s">
-        <v>76</v>
+        <v>19</v>
       </c>
       <c r="C44" t="s">
-        <v>52</v>
+        <v>20</v>
       </c>
       <c r="D44" s="1">
-        <v>45879</v>
+        <v>45800</v>
       </c>
       <c r="E44" t="s">
         <v>8</v>
       </c>
       <c r="F44" t="s">
-        <v>38</v>
+        <v>9</v>
       </c>
       <c r="G44" t="s">
-        <v>10</v>
+        <v>56</v>
       </c>
     </row>
     <row r="45" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A45" t="s">
-        <v>72</v>
+        <v>4</v>
       </c>
       <c r="B45" t="s">
-        <v>77</v>
+        <v>42</v>
       </c>
       <c r="C45" t="s">
-        <v>52</v>
+        <v>48</v>
       </c>
       <c r="D45" s="1">
-        <v>45879</v>
+        <v>45891</v>
       </c>
       <c r="E45" t="s">
         <v>8</v>
       </c>
       <c r="F45" t="s">
-        <v>38</v>
+        <v>9</v>
       </c>
       <c r="G45" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
     </row>
     <row r="46" spans="1:7" x14ac:dyDescent="0.3">
@@ -2062,13 +2916,13 @@
         <v>4</v>
       </c>
       <c r="B46" t="s">
-        <v>78</v>
+        <v>47</v>
       </c>
       <c r="C46" t="s">
-        <v>79</v>
+        <v>48</v>
       </c>
       <c r="D46" s="1">
-        <v>45887</v>
+        <v>45891</v>
       </c>
       <c r="E46" t="s">
         <v>8</v>
@@ -2077,7 +2931,7 @@
         <v>9</v>
       </c>
       <c r="G46" t="s">
-        <v>10</v>
+        <v>37</v>
       </c>
     </row>
     <row r="47" spans="1:7" x14ac:dyDescent="0.3">
@@ -2085,22 +2939,22 @@
         <v>4</v>
       </c>
       <c r="B47" t="s">
-        <v>80</v>
+        <v>46</v>
       </c>
       <c r="C47" t="s">
-        <v>18</v>
+        <v>48</v>
       </c>
       <c r="D47" s="1">
-        <v>45920</v>
+        <v>45891</v>
       </c>
       <c r="E47" t="s">
         <v>8</v>
       </c>
       <c r="F47" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="G47" t="s">
-        <v>10</v>
+        <v>37</v>
       </c>
     </row>
     <row r="48" spans="1:7" x14ac:dyDescent="0.3">
@@ -2108,22 +2962,22 @@
         <v>4</v>
       </c>
       <c r="B48" t="s">
-        <v>85</v>
+        <v>41</v>
       </c>
       <c r="C48" t="s">
-        <v>18</v>
+        <v>48</v>
       </c>
       <c r="D48" s="1">
-        <v>45920</v>
+        <v>45891</v>
       </c>
       <c r="E48" t="s">
         <v>8</v>
       </c>
       <c r="F48" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="G48" t="s">
-        <v>10</v>
+        <v>37</v>
       </c>
     </row>
     <row r="49" spans="1:7" x14ac:dyDescent="0.3">
@@ -2131,22 +2985,22 @@
         <v>4</v>
       </c>
       <c r="B49" t="s">
-        <v>81</v>
+        <v>39</v>
       </c>
       <c r="C49" t="s">
-        <v>18</v>
+        <v>48</v>
       </c>
       <c r="D49" s="1">
-        <v>45920</v>
+        <v>45891</v>
       </c>
       <c r="E49" t="s">
         <v>8</v>
       </c>
       <c r="F49" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="G49" t="s">
-        <v>10</v>
+        <v>37</v>
       </c>
     </row>
     <row r="50" spans="1:7" x14ac:dyDescent="0.3">
@@ -2154,22 +3008,22 @@
         <v>4</v>
       </c>
       <c r="B50" t="s">
-        <v>82</v>
+        <v>38</v>
       </c>
       <c r="C50" t="s">
-        <v>18</v>
+        <v>48</v>
       </c>
       <c r="D50" s="1">
-        <v>45920</v>
+        <v>45891</v>
       </c>
       <c r="E50" t="s">
         <v>8</v>
       </c>
       <c r="F50" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="G50" t="s">
-        <v>10</v>
+        <v>37</v>
       </c>
     </row>
     <row r="51" spans="1:7" x14ac:dyDescent="0.3">
@@ -2177,22 +3031,22 @@
         <v>4</v>
       </c>
       <c r="B51" t="s">
-        <v>84</v>
+        <v>44</v>
       </c>
       <c r="C51" t="s">
-        <v>18</v>
+        <v>48</v>
       </c>
       <c r="D51" s="1">
-        <v>45920</v>
+        <v>45891</v>
       </c>
       <c r="E51" t="s">
         <v>8</v>
       </c>
       <c r="F51" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="G51" t="s">
-        <v>10</v>
+        <v>37</v>
       </c>
     </row>
     <row r="52" spans="1:7" x14ac:dyDescent="0.3">
@@ -2200,22 +3054,22 @@
         <v>4</v>
       </c>
       <c r="B52" t="s">
-        <v>83</v>
+        <v>45</v>
       </c>
       <c r="C52" t="s">
-        <v>18</v>
+        <v>48</v>
       </c>
       <c r="D52" s="1">
-        <v>45920</v>
+        <v>45891</v>
       </c>
       <c r="E52" t="s">
         <v>8</v>
       </c>
       <c r="F52" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="G52" t="s">
-        <v>10</v>
+        <v>37</v>
       </c>
     </row>
     <row r="53" spans="1:7" x14ac:dyDescent="0.3">
@@ -2223,22 +3077,22 @@
         <v>4</v>
       </c>
       <c r="B53" t="s">
-        <v>87</v>
+        <v>43</v>
       </c>
       <c r="C53" t="s">
-        <v>18</v>
+        <v>48</v>
       </c>
       <c r="D53" s="1">
-        <v>45920</v>
+        <v>45891</v>
       </c>
       <c r="E53" t="s">
         <v>8</v>
       </c>
       <c r="F53" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="G53" t="s">
-        <v>10</v>
+        <v>37</v>
       </c>
     </row>
     <row r="54" spans="1:7" x14ac:dyDescent="0.3">
@@ -2246,80 +3100,87 @@
         <v>4</v>
       </c>
       <c r="B54" t="s">
-        <v>86</v>
+        <v>40</v>
       </c>
       <c r="C54" t="s">
-        <v>18</v>
+        <v>48</v>
       </c>
       <c r="D54" s="1">
-        <v>45920</v>
+        <v>45891</v>
       </c>
       <c r="E54" t="s">
         <v>8</v>
       </c>
       <c r="F54" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="G54" t="s">
-        <v>10</v>
+        <v>37</v>
       </c>
     </row>
     <row r="55" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A55" t="s">
-        <v>59</v>
+        <v>4</v>
       </c>
       <c r="B55" t="s">
-        <v>88</v>
+        <v>13</v>
       </c>
       <c r="C55" t="s">
-        <v>37</v>
+        <v>16</v>
       </c>
       <c r="D55" s="1">
-        <v>45921</v>
+        <v>45822</v>
       </c>
       <c r="E55" t="s">
         <v>8</v>
       </c>
       <c r="F55" t="s">
-        <v>38</v>
+        <v>9</v>
       </c>
       <c r="G55" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
     </row>
   </sheetData>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:I55">
+    <sortCondition ref="E2:E55" customList="Done,In Progress,Planned,Not Started"/>
+    <sortCondition ref="F2:F55" customList="Done,In Progress,Planned,Not Started"/>
+    <sortCondition ref="G2:G55" customList="Done,In Progress,Planned,Not Started"/>
+    <sortCondition ref="A2:A55" customList="Goat,Gladiator,Edison,Tengu Plant,HAT,Advanced"/>
+    <sortCondition ref="B2:B55"/>
+  </sortState>
   <conditionalFormatting sqref="A1:A1048576">
-    <cfRule type="cellIs" dxfId="9" priority="2" operator="equal">
+    <cfRule type="cellIs" dxfId="9" priority="26" operator="equal">
       <formula>"Advanced Format"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="8" priority="3" operator="equal">
+    <cfRule type="cellIs" dxfId="8" priority="27" operator="equal">
       <formula>"HAT"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="7" priority="4" operator="equal">
+    <cfRule type="cellIs" dxfId="7" priority="28" operator="equal">
       <formula>"Tengu Plant"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="6" priority="5" operator="equal">
+    <cfRule type="cellIs" dxfId="6" priority="29" operator="equal">
       <formula>"Edison"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="5" priority="6" operator="equal">
+    <cfRule type="cellIs" dxfId="5" priority="30" operator="equal">
       <formula>"Gladiator"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="4" priority="7" operator="equal">
+    <cfRule type="cellIs" dxfId="4" priority="31" operator="equal">
       <formula>"Goat"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E1:G1048576">
     <cfRule type="cellIs" dxfId="3" priority="1" operator="equal">
+      <formula>"Not Started"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="2" priority="2" operator="equal">
       <formula>"Planned"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="2" priority="8" operator="equal">
-      <formula>"Complete"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="1" priority="9" operator="equal">
+    <cfRule type="cellIs" dxfId="1" priority="3" operator="equal">
       <formula>"In Progress"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="0" priority="10" operator="equal">
-      <formula>"Not Started"</formula>
+    <cfRule type="cellIs" dxfId="0" priority="8" operator="equal">
+      <formula>"Done"</formula>
     </cfRule>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>